<commit_message>
bulk update rest api
</commit_message>
<xml_diff>
--- a/scrubFolder/bulkPref.xlsx
+++ b/scrubFolder/bulkPref.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -209,16 +209,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA1" activeCellId="0" sqref="AA1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -317,7 +314,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>9898989898</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -412,7 +409,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>9898989898</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -502,6 +499,291 @@
         <v>1</v>
       </c>
       <c r="AE3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pages linked, bulk consents and bulk preferences complete
</commit_message>
<xml_diff>
--- a/scrubFolder/bulkPref.xlsx
+++ b/scrubFolder/bulkPref.xlsx
@@ -224,16 +224,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,19 +411,19 @@
         <v>1</v>
       </c>
       <c r="AA2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AC2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1" t="n">
         <v>1</v>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="Y3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="1" t="n">
         <v>1</v>
@@ -540,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>1</v>
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1" t="n">
         <v>1</v>
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" s="1" t="n">
         <v>1</v>
@@ -597,22 +597,22 @@
         <v>1</v>
       </c>
       <c r="Y4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AA4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AD4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="1" t="n">
         <v>1</v>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>1</v>
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>1</v>
@@ -672,13 +672,13 @@
         <v>1</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" s="1" t="n">
         <v>1</v>
@@ -693,16 +693,16 @@
         <v>1</v>
       </c>
       <c r="Y5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="1" t="n">
         <v>1</v>
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -735,13 +735,13 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>1</v>
@@ -795,10 +795,10 @@
         <v>1</v>
       </c>
       <c r="AA6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="1" t="n">
         <v>1</v>
@@ -810,9 +810,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>2</v>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>9123456800</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
@@ -836,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>1</v>
@@ -851,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1" t="n">
         <v>1</v>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" s="1" t="n">
         <v>1</v>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="Z7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="1" t="n">
         <v>1</v>
@@ -896,24 +896,24 @@
         <v>1</v>
       </c>
       <c r="AC7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AE7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>3</v>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>9123456793</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -934,13 +934,13 @@
         <v>1</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>1</v>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="U8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" s="1" t="n">
         <v>1</v>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="AA8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="1" t="n">
         <v>1</v>
@@ -994,24 +994,25 @@
         <v>1</v>
       </c>
       <c r="AD8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>6</v>
+      <c r="A9" s="0" t="n">
+        <f aca="false">A8+5</f>
+        <v>9123456798</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>1</v>
@@ -1035,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>1</v>
@@ -1047,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
         <v>1</v>
@@ -1059,13 +1060,13 @@
         <v>1</v>
       </c>
       <c r="T9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="n">
         <v>1</v>
@@ -1074,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="Y9" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="1" t="n">
         <v>1</v>
@@ -1096,8 +1097,9 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" s="0" t="n">
+        <f aca="false">A9+5</f>
+        <v>9123456803</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
@@ -1151,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="1" t="n">
         <v>1</v>
@@ -1181,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="AC10" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="1" t="n">
         <v>1</v>
@@ -1191,8 +1193,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
+      <c r="A11" s="0" t="n">
+        <f aca="false">A10+5</f>
+        <v>9123456808</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>1</v>
@@ -1249,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="T11" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="1" t="n">
         <v>1</v>
@@ -1273,16 +1276,1158 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AD11" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <f aca="false">A11+5</f>
+        <v>9123456813</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>9123456794</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <f aca="false">A13+5</f>
+        <v>9123456799</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>9223456802</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>9223456803</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>9223456804</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>9223456805</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>9223456806</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>9223456807</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>9223456808</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>9223456809</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>9223456810</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User Complaint filing backend updated
</commit_message>
<xml_diff>
--- a/scrubFolder/bulkPref.xlsx
+++ b/scrubFolder/bulkPref.xlsx
@@ -227,13 +227,13 @@
   <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +333,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>9123456789</v>
+        <v>9012345678</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
@@ -426,10 +426,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <f aca="false">A2+5</f>
-        <v>9123456794</v>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>9012345679</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -522,10 +521,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <f aca="false">A3+5</f>
-        <v>9123456799</v>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>9012345680</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1</v>
@@ -618,10 +616,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <f aca="false">A4+5</f>
-        <v>9123456804</v>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>9012345681</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1</v>
@@ -714,10 +711,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <f aca="false">A5+5</f>
-        <v>9123456809</v>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>9012345682</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -812,7 +808,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>9123456800</v>
+        <v>9012345683</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
@@ -907,7 +903,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>9123456793</v>
+        <v>9012345684</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
@@ -1000,10 +996,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <f aca="false">A8+5</f>
-        <v>9123456798</v>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>9012345685</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
@@ -1096,10 +1091,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <f aca="false">A9+5</f>
-        <v>9123456803</v>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>9012345686</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
@@ -1192,10 +1186,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <f aca="false">A10+5</f>
-        <v>9123456808</v>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>9012345687</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>1</v>
@@ -1288,10 +1281,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <f aca="false">A11+5</f>
-        <v>9123456813</v>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>9012345688</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1</v>
@@ -1386,7 +1378,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>9123456794</v>
+        <v>9012345689</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1</v>
@@ -1479,10 +1471,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <f aca="false">A13+5</f>
-        <v>9123456799</v>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>9012345690</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>1</v>
@@ -1577,7 +1568,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>9223456802</v>
+        <v>9012345691</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>1</v>
@@ -1672,7 +1663,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>9223456803</v>
+        <v>9012345692</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>1</v>
@@ -1767,7 +1758,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>9223456804</v>
+        <v>9012345693</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
@@ -1862,7 +1853,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>9223456805</v>
+        <v>9012345694</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>1</v>
@@ -1957,7 +1948,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>9223456806</v>
+        <v>9012345695</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>1</v>
@@ -2052,7 +2043,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>9223456807</v>
+        <v>9012345696</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>1</v>
@@ -2147,7 +2138,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>9223456808</v>
+        <v>9012345697</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>1</v>
@@ -2242,7 +2233,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>9223456809</v>
+        <v>9012345698</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>1</v>
@@ -2337,7 +2328,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>9223456810</v>
+        <v>9012345699</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1</v>

</xml_diff>